<commit_message>
Battery.xls adjust value with the correct power bank.
</commit_message>
<xml_diff>
--- a/Documentation/Kit/Calcul autonomie/Battery.xlsx
+++ b/Documentation/Kit/Calcul autonomie/Battery.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\rayho\Documentations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\rayho\NewGit\DIY_PM\Documentation\Kit\Calcul autonomie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AF6FDB-627D-4458-AD6D-4C119CD1FACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B5F6AF-2064-4B09-A9C1-DA5340EEA932}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,6 +457,12 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -464,12 +470,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,8 +691,8 @@
   </sheetPr>
   <dimension ref="A1:Z1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -912,7 +912,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="9">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>10</v>
@@ -980,7 +980,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="9">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>10</v>
@@ -1016,7 +1016,7 @@
       <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="48">
+      <c r="B10" s="44">
         <v>0.2</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1051,17 +1051,17 @@
         <v>35</v>
       </c>
       <c r="B11" s="14">
-        <v>5760</v>
+        <v>1440</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="48">
-        <f>(3600 / 15) * 24</f>
-        <v>5760</v>
+      <c r="E11" s="44">
+        <f>(3600 / 60) * 24</f>
+        <v>1440</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -1153,11 +1153,11 @@
       </c>
       <c r="B14" s="19">
         <f>B7*B2/3600</f>
-        <v>3.3333333333333335</v>
+        <v>3</v>
       </c>
       <c r="C14" s="20">
         <f>B14*B3</f>
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="12"/>
@@ -1260,11 +1260,11 @@
       </c>
       <c r="B17" s="24">
         <f>B9*B10/3600</f>
-        <v>1.6666666666666666E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="C17" s="25">
         <f>B17*B11</f>
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="27"/>
@@ -1319,12 +1319,12 @@
       <c r="Z18" s="5"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="46" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="30">
         <f>C14+C15+C16+C17</f>
-        <v>302.834</v>
+        <v>210.834</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>24</v>
@@ -1354,10 +1354,10 @@
       <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="45"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="32">
         <f>B19*30</f>
-        <v>9085.02</v>
+        <v>6325.02</v>
       </c>
       <c r="C20" s="33" t="s">
         <v>25</v>
@@ -1387,10 +1387,10 @@
       <c r="Z20" s="5"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="46"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="35">
         <f>B19*365</f>
-        <v>110534.41</v>
+        <v>76954.41</v>
       </c>
       <c r="C21" s="36" t="s">
         <v>26</v>
@@ -1480,7 +1480,7 @@
         <v>27</v>
       </c>
       <c r="B24" s="7">
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="C24" s="37" t="s">
         <v>28</v>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="B25" s="35">
         <f>B24/(1.1*1.2*1.15)</f>
-        <v>9881.422924901186</v>
+        <v>13175.230566534914</v>
       </c>
       <c r="C25" s="39" t="s">
         <v>28</v>
@@ -1575,12 +1575,12 @@
       <c r="Z26" s="5"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="49" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="40">
         <f>B25/B19</f>
-        <v>32.629833258158548</v>
+        <v>62.491014573242047</v>
       </c>
       <c r="C27" s="37" t="s">
         <v>32</v>
@@ -1610,10 +1610,10 @@
       <c r="Z27" s="5"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="45"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="41">
         <f>B25/B20</f>
-        <v>1.087661108605285</v>
+        <v>2.083033819108068</v>
       </c>
       <c r="C28" s="42" t="s">
         <v>33</v>
@@ -1643,10 +1643,10 @@
       <c r="Z28" s="5"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
+      <c r="A29" s="48"/>
       <c r="B29" s="43">
         <f>B25/B21</f>
-        <v>8.9396803447009718E-2</v>
+        <v>0.17120825910477272</v>
       </c>
       <c r="C29" s="39" t="s">
         <v>34</v>

</xml_diff>